<commit_message>
fix circular imports and tests
</commit_message>
<xml_diff>
--- a/tests/edb/data/areasources.xlsx
+++ b/tests/edb/data/areasources.xlsx
@@ -506,10 +506,10 @@
   <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.09"/>
@@ -605,7 +605,9 @@
       <c r="D3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1" t="n">
+        <v>3857</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
         <v>16</v>
@@ -639,7 +641,9 @@
       <c r="D4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="n">
+        <v>3857</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
         <v>16</v>
@@ -671,7 +675,9 @@
       <c r="D5" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="n">
+        <v>3857</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
@@ -744,10 +750,10 @@
   <dimension ref="A1:N54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="1" sqref="E5 A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -2238,10 +2244,10 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E5 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.17"/>
@@ -2301,10 +2307,10 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="E5 D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.06"/>

</xml_diff>

<commit_message>
fix bug related to facility None
</commit_message>
<xml_diff>
--- a/tests/edb/data/areasources.xlsx
+++ b/tests/edb/data/areasources.xlsx
@@ -506,10 +506,10 @@
   <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+      <selection pane="topLeft" activeCell="P33" activeCellId="0" sqref="P33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.09"/>
@@ -753,7 +753,7 @@
       <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -2247,7 +2247,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.17"/>
@@ -2310,7 +2310,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.06"/>

</xml_diff>